<commit_message>
BASIC_EN vocabulary fixes; some study list navigation fixed
</commit_message>
<xml_diff>
--- a/RES/XLS/TEST_VOCABULARY_FOR _PROJECT.xlsx
+++ b/RES/XLS/TEST_VOCABULARY_FOR _PROJECT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00 MY\00_PROJECTS\00_BETROOT_PROJECT\RES\XLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40043C80-5259-41D9-A265-03469ED1A580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E32788A-297D-454F-A0DB-D5AE730BF36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1372,7 +1372,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1577,6 +1577,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1808,7 +1811,7 @@
   <dimension ref="A1:AC111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
@@ -1882,93 +1885,89 @@
     </row>
     <row r="2" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="64">
-        <v>915</v>
-      </c>
-      <c r="B2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="F2" s="65" t="s">
-        <v>257</v>
-      </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="I2" s="68" t="s">
-        <v>326</v>
-      </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="31" t="s">
-        <v>358</v>
-      </c>
-      <c r="L2" s="20"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="21"/>
-    </row>
-    <row r="3" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>294</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="28"/>
+      <c r="E2" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="69" t="s">
+        <v>265</v>
+      </c>
+      <c r="J2" s="26"/>
+      <c r="K2" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="L2" s="23"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="29"/>
+    </row>
+    <row r="3" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="64">
-        <v>922</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="I3" s="68" t="s">
-        <v>327</v>
-      </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="31" t="s">
-        <v>358</v>
-      </c>
-      <c r="L3" s="20"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="21"/>
-    </row>
-    <row r="4" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="28"/>
+      <c r="E3" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="23"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="69"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="L3" s="23"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="29"/>
+    </row>
+    <row r="4" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="64">
-        <v>924</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>1</v>
+        <v>237</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="C4" s="67" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="24" t="s">
-        <v>161</v>
+        <v>235</v>
       </c>
       <c r="F4" s="23"/>
       <c r="G4" s="24"/>
-      <c r="H4" s="32" t="s">
-        <v>162</v>
+      <c r="H4" s="25" t="s">
+        <v>236</v>
       </c>
       <c r="I4" s="69" t="s">
-        <v>328</v>
+        <v>280</v>
       </c>
       <c r="J4" s="26"/>
-      <c r="K4" s="31" t="s">
-        <v>358</v>
+      <c r="K4" s="33" t="s">
+        <v>237</v>
       </c>
       <c r="L4" s="23"/>
       <c r="M4" s="28"/>
@@ -1977,29 +1976,29 @@
     </row>
     <row r="5" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="64">
-        <v>936</v>
-      </c>
-      <c r="B5" s="48" t="s">
-        <v>1</v>
+        <v>825</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="C5" s="67" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="28"/>
-      <c r="E5" s="24" t="s">
-        <v>163</v>
+      <c r="E5" s="44" t="s">
+        <v>140</v>
       </c>
       <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
+      <c r="G5" s="44"/>
       <c r="H5" s="32" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
       <c r="I5" s="69" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="J5" s="26"/>
-      <c r="K5" s="31" t="s">
-        <v>358</v>
+      <c r="K5" s="33" t="s">
+        <v>142</v>
       </c>
       <c r="L5" s="23"/>
       <c r="M5" s="28"/>
@@ -2008,9 +2007,9 @@
     </row>
     <row r="6" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="64">
-        <v>29</v>
-      </c>
-      <c r="B6" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="66" t="s">
@@ -2018,110 +2017,112 @@
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="15" t="s">
-        <v>44</v>
+        <v>221</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="15"/>
       <c r="H6" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="17"/>
+        <v>222</v>
+      </c>
+      <c r="I6" s="68" t="s">
+        <v>269</v>
+      </c>
       <c r="J6" s="18"/>
-      <c r="K6" s="31" t="s">
-        <v>358</v>
+      <c r="K6" s="19" t="s">
+        <v>223</v>
       </c>
       <c r="L6" s="20"/>
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
       <c r="O6" s="21"/>
     </row>
-    <row r="7" spans="1:15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="64">
-        <v>949</v>
-      </c>
-      <c r="B7" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="28"/>
+        <v>2644</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="34"/>
       <c r="E7" s="24" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
-      <c r="H7" s="32" t="s">
-        <v>166</v>
+      <c r="H7" s="25" t="s">
+        <v>26</v>
       </c>
       <c r="I7" s="69" t="s">
-        <v>330</v>
+        <v>351</v>
       </c>
       <c r="J7" s="26"/>
-      <c r="K7" s="31" t="s">
-        <v>358</v>
+      <c r="K7" s="33" t="s">
+        <v>27</v>
       </c>
       <c r="L7" s="23"/>
       <c r="M7" s="28"/>
       <c r="N7" s="28"/>
       <c r="O7" s="29"/>
     </row>
-    <row r="8" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="64">
-        <v>31</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="24" t="s">
-        <v>210</v>
-      </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25" t="s">
-        <v>211</v>
-      </c>
-      <c r="I8" s="69" t="s">
-        <v>258</v>
-      </c>
-      <c r="J8" s="26"/>
-      <c r="K8" s="31" t="s">
-        <v>358</v>
-      </c>
-      <c r="L8" s="23"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="29"/>
-    </row>
-    <row r="9" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1011</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="I8" s="68" t="s">
+        <v>336</v>
+      </c>
+      <c r="J8" s="18"/>
+      <c r="K8" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="L8" s="20"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="21"/>
+    </row>
+    <row r="9" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="64">
-        <v>966</v>
-      </c>
-      <c r="B9" s="48" t="s">
-        <v>1</v>
+        <v>318</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="14"/>
-      <c r="E9" s="36" t="s">
-        <v>167</v>
+      <c r="E9" s="15" t="s">
+        <v>238</v>
       </c>
       <c r="F9" s="20"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="52" t="s">
-        <v>168</v>
+      <c r="G9" s="15"/>
+      <c r="H9" s="30" t="s">
+        <v>239</v>
       </c>
       <c r="I9" s="68" t="s">
-        <v>331</v>
-      </c>
-      <c r="J9" s="39"/>
-      <c r="K9" s="31" t="s">
-        <v>358</v>
+        <v>266</v>
+      </c>
+      <c r="J9" s="18"/>
+      <c r="K9" s="19" t="s">
+        <v>240</v>
       </c>
       <c r="L9" s="20"/>
       <c r="M9" s="14"/>
@@ -2130,7 +2131,7 @@
     </row>
     <row r="10" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="64">
-        <v>972</v>
+        <v>1076</v>
       </c>
       <c r="B10" s="48" t="s">
         <v>1</v>
@@ -2139,20 +2140,20 @@
         <v>5</v>
       </c>
       <c r="D10" s="28"/>
-      <c r="E10" s="40" t="s">
-        <v>169</v>
+      <c r="E10" s="24" t="s">
+        <v>193</v>
       </c>
       <c r="F10" s="23"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="56" t="s">
-        <v>170</v>
+      <c r="G10" s="24"/>
+      <c r="H10" s="32" t="s">
+        <v>194</v>
       </c>
       <c r="I10" s="69" t="s">
-        <v>332</v>
-      </c>
-      <c r="J10" s="41"/>
-      <c r="K10" s="31" t="s">
-        <v>358</v>
+        <v>343</v>
+      </c>
+      <c r="J10" s="26"/>
+      <c r="K10" s="33" t="s">
+        <v>195</v>
       </c>
       <c r="L10" s="23"/>
       <c r="M10" s="28"/>
@@ -2161,94 +2162,100 @@
     </row>
     <row r="11" spans="1:15" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="64">
-        <v>975</v>
-      </c>
-      <c r="B11" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="28"/>
+      <c r="E11" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="69" t="s">
+        <v>278</v>
+      </c>
+      <c r="J11" s="26"/>
+      <c r="K11" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="23"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="29"/>
+    </row>
+    <row r="12" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="64">
+        <v>1091</v>
+      </c>
+      <c r="B12" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="43" t="s">
-        <v>171</v>
-      </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="52" t="s">
-        <v>172</v>
-      </c>
-      <c r="I11" s="68" t="s">
-        <v>333</v>
-      </c>
-      <c r="J11" s="43"/>
-      <c r="K11" s="31" t="s">
-        <v>358</v>
-      </c>
-      <c r="L11" s="20"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="21"/>
-    </row>
-    <row r="12" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="64">
-        <v>55</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="38"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="21"/>
+      <c r="C12" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12" s="23"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="I12" s="69" t="s">
+        <v>345</v>
+      </c>
+      <c r="J12" s="26"/>
+      <c r="K12" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="L12" s="23"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="29"/>
     </row>
     <row r="13" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="64">
-        <v>979</v>
-      </c>
-      <c r="B13" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="55" t="s">
-        <v>173</v>
-      </c>
-      <c r="F13" s="23"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="56" t="s">
-        <v>156</v>
-      </c>
-      <c r="I13" s="69" t="s">
-        <v>319</v>
-      </c>
-      <c r="J13" s="55"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="29"/>
-    </row>
-    <row r="14" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="F13" s="20"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="I13" s="68" t="s">
+        <v>267</v>
+      </c>
+      <c r="J13" s="18"/>
+      <c r="K13" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="L13" s="20"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="21"/>
+    </row>
+    <row r="14" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="64">
-        <v>59</v>
+        <v>199</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>0</v>
@@ -2258,18 +2265,20 @@
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="24" t="s">
-        <v>215</v>
+        <v>20</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
-      <c r="H14" s="25" t="s">
-        <v>216</v>
+      <c r="H14" s="32" t="s">
+        <v>21</v>
       </c>
       <c r="I14" s="69" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="J14" s="26"/>
-      <c r="K14" s="27"/>
+      <c r="K14" s="33" t="s">
+        <v>22</v>
+      </c>
       <c r="L14" s="23"/>
       <c r="M14" s="28"/>
       <c r="N14" s="28"/>
@@ -2277,36 +2286,38 @@
     </row>
     <row r="15" spans="1:15" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="64">
-        <v>983</v>
-      </c>
-      <c r="B15" s="48" t="s">
-        <v>1</v>
+        <v>261</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="15" t="s">
-        <v>174</v>
+        <v>129</v>
       </c>
       <c r="F15" s="20"/>
       <c r="G15" s="15"/>
       <c r="H15" s="16" t="s">
-        <v>175</v>
+        <v>130</v>
       </c>
       <c r="I15" s="68" t="s">
-        <v>334</v>
+        <v>281</v>
       </c>
       <c r="J15" s="18"/>
-      <c r="K15" s="31"/>
+      <c r="K15" s="19" t="s">
+        <v>359</v>
+      </c>
       <c r="L15" s="20"/>
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
       <c r="O15" s="21"/>
     </row>
-    <row r="16" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="64">
-        <v>72</v>
+        <v>262</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>0</v>
@@ -2316,28 +2327,28 @@
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="15" t="s">
-        <v>221</v>
+        <v>131</v>
       </c>
       <c r="F16" s="20"/>
       <c r="G16" s="15"/>
-      <c r="H16" s="30" t="s">
-        <v>222</v>
+      <c r="H16" s="16" t="s">
+        <v>132</v>
       </c>
       <c r="I16" s="68" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="J16" s="18"/>
       <c r="K16" s="19" t="s">
-        <v>223</v>
+        <v>359</v>
       </c>
       <c r="L16" s="20"/>
       <c r="M16" s="14"/>
       <c r="N16" s="14"/>
       <c r="O16" s="21"/>
     </row>
-    <row r="17" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="64">
-        <v>88</v>
+        <v>264</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>0</v>
@@ -2347,18 +2358,20 @@
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="15" t="s">
-        <v>227</v>
+        <v>135</v>
       </c>
       <c r="F17" s="20"/>
       <c r="G17" s="15"/>
-      <c r="H17" s="30" t="s">
-        <v>57</v>
+      <c r="H17" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="I17" s="68" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J17" s="18"/>
-      <c r="K17" s="19"/>
+      <c r="K17" s="19" t="s">
+        <v>359</v>
+      </c>
       <c r="L17" s="20"/>
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>
@@ -2366,36 +2379,38 @@
     </row>
     <row r="18" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="64">
-        <v>93</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="F18" s="20"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="30" t="s">
-        <v>229</v>
-      </c>
-      <c r="I18" s="68" t="s">
-        <v>270</v>
-      </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="21"/>
-    </row>
-    <row r="19" spans="1:15" customFormat="1" ht="31" x14ac:dyDescent="0.25">
+        <v>2895</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="F18" s="23"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="I18" s="69" t="s">
+        <v>353</v>
+      </c>
+      <c r="J18" s="26"/>
+      <c r="K18" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="L18" s="23"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="29"/>
+    </row>
+    <row r="19" spans="1:15" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A19" s="64">
-        <v>95</v>
+        <v>271</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>0</v>
@@ -2405,17 +2420,19 @@
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="24" t="s">
-        <v>77</v>
+        <v>136</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
-      <c r="H19" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="I19" s="69"/>
+      <c r="H19" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="I19" s="69" t="s">
+        <v>283</v>
+      </c>
       <c r="J19" s="26"/>
-      <c r="K19" s="33" t="s">
-        <v>79</v>
+      <c r="K19" s="19" t="s">
+        <v>359</v>
       </c>
       <c r="L19" s="23"/>
       <c r="M19" s="28"/>
@@ -2424,7 +2441,7 @@
     </row>
     <row r="20" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="64">
-        <v>96</v>
+        <v>272</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>0</v>
@@ -2434,55 +2451,59 @@
       </c>
       <c r="D20" s="28"/>
       <c r="E20" s="24" t="s">
-        <v>230</v>
-      </c>
-      <c r="F20" s="23"/>
+        <v>62</v>
+      </c>
+      <c r="F20" s="34"/>
       <c r="G20" s="24"/>
       <c r="H20" s="25" t="s">
-        <v>231</v>
+        <v>63</v>
       </c>
       <c r="I20" s="69" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="J20" s="26"/>
-      <c r="K20" s="33"/>
-      <c r="L20" s="23"/>
+      <c r="K20" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="L20" s="34"/>
       <c r="M20" s="28"/>
       <c r="N20" s="28"/>
       <c r="O20" s="29"/>
     </row>
-    <row r="21" spans="1:15" customFormat="1" ht="28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="64">
-        <v>101</v>
+        <v>274</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="67" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="23"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="I21" s="69" t="s">
-        <v>272</v>
-      </c>
-      <c r="J21" s="26"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="29"/>
-    </row>
-    <row r="22" spans="1:15" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="20"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" s="68" t="s">
+        <v>264</v>
+      </c>
+      <c r="J21" s="18"/>
+      <c r="K21" s="19" t="s">
+        <v>359</v>
+      </c>
+      <c r="L21" s="20"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="21"/>
+    </row>
+    <row r="22" spans="1:15" customFormat="1" ht="28" x14ac:dyDescent="0.35">
       <c r="A22" s="64">
-        <v>102</v>
+        <v>275</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>0</v>
@@ -2492,107 +2513,113 @@
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="15" t="s">
-        <v>6</v>
+        <v>138</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="15"/>
       <c r="H22" s="16" t="s">
-        <v>7</v>
+        <v>139</v>
       </c>
       <c r="I22" s="68" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
+      <c r="K22" s="19" t="s">
+        <v>359</v>
+      </c>
       <c r="L22" s="20"/>
       <c r="M22" s="14"/>
       <c r="N22" s="14"/>
       <c r="O22" s="21"/>
     </row>
-    <row r="23" spans="1:15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="64">
-        <v>1010</v>
-      </c>
-      <c r="B23" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="66" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="I23" s="68" t="s">
-        <v>335</v>
-      </c>
-      <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="21"/>
-    </row>
-    <row r="24" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+        <v>3562</v>
+      </c>
+      <c r="B23" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="28"/>
+      <c r="E23" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="F23" s="23"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="I23" s="69" t="s">
+        <v>356</v>
+      </c>
+      <c r="J23" s="26"/>
+      <c r="K23" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="L23" s="23"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="29"/>
+    </row>
+    <row r="24" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="64">
-        <v>1011</v>
-      </c>
-      <c r="B24" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="14"/>
-      <c r="E24" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="16" t="s">
-        <v>179</v>
-      </c>
-      <c r="I24" s="68" t="s">
-        <v>336</v>
-      </c>
-      <c r="J24" s="18"/>
-      <c r="K24" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="L24" s="20"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="21"/>
+        <v>3057</v>
+      </c>
+      <c r="B24" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="23"/>
+      <c r="E24" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="F24" s="23"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="I24" s="69" t="s">
+        <v>354</v>
+      </c>
+      <c r="J24" s="24"/>
+      <c r="K24" s="33" t="s">
+        <v>234</v>
+      </c>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="57"/>
     </row>
     <row r="25" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="64">
-        <v>1012</v>
-      </c>
-      <c r="B25" s="48" t="s">
-        <v>1</v>
+        <v>459</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="15" t="s">
-        <v>181</v>
+        <v>80</v>
       </c>
       <c r="F25" s="20"/>
       <c r="G25" s="15"/>
       <c r="H25" s="16" t="s">
-        <v>182</v>
+        <v>81</v>
       </c>
       <c r="I25" s="68" t="s">
-        <v>337</v>
+        <v>293</v>
       </c>
       <c r="J25" s="18"/>
-      <c r="K25" s="19"/>
+      <c r="K25" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="L25" s="20"/>
       <c r="M25" s="14"/>
       <c r="N25" s="14"/>
@@ -2600,36 +2627,38 @@
     </row>
     <row r="26" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="64">
-        <v>119</v>
+        <v>731</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="68" t="s">
-        <v>274</v>
-      </c>
-      <c r="J26" s="18"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="21"/>
+      <c r="C26" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="28"/>
+      <c r="E26" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="F26" s="23"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="I26" s="69" t="s">
+        <v>316</v>
+      </c>
+      <c r="J26" s="26"/>
+      <c r="K26" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="L26" s="23"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="29"/>
     </row>
     <row r="27" spans="1:15" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="64">
-        <v>1023</v>
+        <v>1714</v>
       </c>
       <c r="B27" s="48" t="s">
         <v>1</v>
@@ -2639,47 +2668,53 @@
       </c>
       <c r="D27" s="28"/>
       <c r="E27" s="24" t="s">
-        <v>183</v>
+        <v>207</v>
       </c>
       <c r="F27" s="23"/>
       <c r="G27" s="24"/>
       <c r="H27" s="32" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="I27" s="69" t="s">
-        <v>338</v>
+        <v>349</v>
       </c>
       <c r="J27" s="26"/>
-      <c r="K27" s="33"/>
+      <c r="K27" s="33" t="s">
+        <v>209</v>
+      </c>
       <c r="L27" s="23"/>
       <c r="M27" s="28"/>
       <c r="N27" s="28"/>
       <c r="O27" s="29"/>
     </row>
-    <row r="28" spans="1:15" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" customFormat="1" ht="35.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="64">
-        <v>1035</v>
-      </c>
-      <c r="B28" s="48" t="s">
-        <v>1</v>
+        <v>2283</v>
+      </c>
+      <c r="B28" s="50" t="s">
+        <v>2</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="28"/>
       <c r="E28" s="24" t="s">
-        <v>185</v>
+        <v>30</v>
       </c>
       <c r="F28" s="23"/>
       <c r="G28" s="24"/>
-      <c r="H28" s="32" t="s">
-        <v>186</v>
+      <c r="H28" s="25" t="s">
+        <v>31</v>
       </c>
       <c r="I28" s="69" t="s">
-        <v>339</v>
-      </c>
-      <c r="J28" s="26"/>
-      <c r="K28" s="33"/>
+        <v>315</v>
+      </c>
+      <c r="J28" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="K28" s="33" t="s">
+        <v>8</v>
+      </c>
       <c r="L28" s="23"/>
       <c r="M28" s="28"/>
       <c r="N28" s="28"/>
@@ -2687,57 +2722,63 @@
     </row>
     <row r="29" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="64">
-        <v>1048</v>
-      </c>
-      <c r="B29" s="48" t="s">
-        <v>1</v>
+        <v>167</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D29" s="14"/>
       <c r="E29" s="15" t="s">
-        <v>187</v>
+        <v>17</v>
       </c>
       <c r="F29" s="20"/>
       <c r="G29" s="15"/>
       <c r="H29" s="16" t="s">
-        <v>188</v>
+        <v>18</v>
       </c>
       <c r="I29" s="68" t="s">
-        <v>340</v>
+        <v>276</v>
       </c>
       <c r="J29" s="18"/>
-      <c r="K29" s="19"/>
+      <c r="K29" s="19" t="s">
+        <v>19</v>
+      </c>
       <c r="L29" s="20"/>
       <c r="M29" s="14"/>
       <c r="N29" s="14"/>
       <c r="O29" s="21"/>
     </row>
-    <row r="30" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="64">
-        <v>154</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>0</v>
+        <v>915</v>
+      </c>
+      <c r="B30" s="48" t="s">
+        <v>1</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="14"/>
       <c r="E30" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="20"/>
+        <v>157</v>
+      </c>
+      <c r="F30" s="65" t="s">
+        <v>257</v>
+      </c>
       <c r="G30" s="15"/>
-      <c r="H30" s="46" t="s">
-        <v>10</v>
+      <c r="H30" s="16" t="s">
+        <v>158</v>
       </c>
       <c r="I30" s="68" t="s">
-        <v>275</v>
+        <v>326</v>
       </c>
       <c r="J30" s="18"/>
-      <c r="K30" s="19"/>
+      <c r="K30" s="31" t="s">
+        <v>358</v>
+      </c>
       <c r="L30" s="20"/>
       <c r="M30" s="14"/>
       <c r="N30" s="14"/>
@@ -2745,127 +2786,129 @@
     </row>
     <row r="31" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="64">
-        <v>1054</v>
+        <v>922</v>
       </c>
       <c r="B31" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="28"/>
-      <c r="E31" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="F31" s="23"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="32" t="s">
-        <v>190</v>
-      </c>
-      <c r="I31" s="69" t="s">
-        <v>341</v>
-      </c>
-      <c r="J31" s="26"/>
-      <c r="K31" s="33"/>
-      <c r="L31" s="23"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="28"/>
-      <c r="O31" s="29"/>
+      <c r="C31" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="14"/>
+      <c r="E31" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="F31" s="20"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="I31" s="68" t="s">
+        <v>327</v>
+      </c>
+      <c r="J31" s="18"/>
+      <c r="K31" s="31" t="s">
+        <v>358</v>
+      </c>
+      <c r="L31" s="20"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="21"/>
     </row>
     <row r="32" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="64">
-        <v>1065</v>
+        <v>924</v>
       </c>
       <c r="B32" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="I32" s="68" t="s">
-        <v>342</v>
-      </c>
-      <c r="J32" s="18"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="21"/>
+      <c r="C32" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="28"/>
+      <c r="E32" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="F32" s="23"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="I32" s="69" t="s">
+        <v>328</v>
+      </c>
+      <c r="J32" s="26"/>
+      <c r="K32" s="31" t="s">
+        <v>358</v>
+      </c>
+      <c r="L32" s="23"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="29"/>
     </row>
     <row r="33" spans="1:15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="64">
-        <v>167</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="20"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="I33" s="68" t="s">
-        <v>276</v>
-      </c>
-      <c r="J33" s="18"/>
-      <c r="K33" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="L33" s="20"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="21"/>
+        <v>936</v>
+      </c>
+      <c r="B33" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="28"/>
+      <c r="E33" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="F33" s="23"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="I33" s="69" t="s">
+        <v>329</v>
+      </c>
+      <c r="J33" s="26"/>
+      <c r="K33" s="31" t="s">
+        <v>358</v>
+      </c>
+      <c r="L33" s="23"/>
+      <c r="M33" s="28"/>
+      <c r="N33" s="28"/>
+      <c r="O33" s="29"/>
     </row>
     <row r="34" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="64">
-        <v>2644</v>
-      </c>
-      <c r="B34" s="51" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="34"/>
-      <c r="E34" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="F34" s="23"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="I34" s="69" t="s">
-        <v>351</v>
-      </c>
-      <c r="J34" s="26"/>
-      <c r="K34" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="L34" s="23"/>
-      <c r="M34" s="28"/>
-      <c r="N34" s="28"/>
-      <c r="O34" s="29"/>
+        <v>29</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="14"/>
+      <c r="E34" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="20"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="I34" s="17"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="31" t="s">
+        <v>358</v>
+      </c>
+      <c r="L34" s="20"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
+      <c r="O34" s="21"/>
     </row>
     <row r="35" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="64">
-        <v>1076</v>
+        <v>949</v>
       </c>
       <c r="B35" s="48" t="s">
         <v>1</v>
@@ -2875,49 +2918,51 @@
       </c>
       <c r="D35" s="28"/>
       <c r="E35" s="24" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="F35" s="23"/>
       <c r="G35" s="24"/>
       <c r="H35" s="32" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="I35" s="69" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="J35" s="26"/>
-      <c r="K35" s="33" t="s">
-        <v>195</v>
+      <c r="K35" s="31" t="s">
+        <v>358</v>
       </c>
       <c r="L35" s="23"/>
       <c r="M35" s="28"/>
       <c r="N35" s="28"/>
       <c r="O35" s="29"/>
     </row>
-    <row r="36" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="64">
-        <v>1090</v>
-      </c>
-      <c r="B36" s="48" t="s">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>0</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="28"/>
       <c r="E36" s="24" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="F36" s="23"/>
       <c r="G36" s="24"/>
-      <c r="H36" s="32" t="s">
-        <v>197</v>
+      <c r="H36" s="25" t="s">
+        <v>211</v>
       </c>
       <c r="I36" s="69" t="s">
-        <v>344</v>
+        <v>258</v>
       </c>
       <c r="J36" s="26"/>
-      <c r="K36" s="33"/>
+      <c r="K36" s="31" t="s">
+        <v>358</v>
+      </c>
       <c r="L36" s="23"/>
       <c r="M36" s="28"/>
       <c r="N36" s="28"/>
@@ -2925,59 +2970,61 @@
     </row>
     <row r="37" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="64">
-        <v>1091</v>
+        <v>966</v>
       </c>
       <c r="B37" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="28"/>
-      <c r="E37" s="24" t="s">
-        <v>198</v>
-      </c>
-      <c r="F37" s="23"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="32" t="s">
-        <v>199</v>
-      </c>
-      <c r="I37" s="69" t="s">
-        <v>345</v>
-      </c>
-      <c r="J37" s="26"/>
-      <c r="K37" s="33" t="s">
-        <v>200</v>
-      </c>
-      <c r="L37" s="23"/>
-      <c r="M37" s="28"/>
-      <c r="N37" s="28"/>
-      <c r="O37" s="29"/>
+      <c r="C37" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="14"/>
+      <c r="E37" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="F37" s="20"/>
+      <c r="G37" s="36"/>
+      <c r="H37" s="52" t="s">
+        <v>168</v>
+      </c>
+      <c r="I37" s="68" t="s">
+        <v>331</v>
+      </c>
+      <c r="J37" s="39"/>
+      <c r="K37" s="31" t="s">
+        <v>358</v>
+      </c>
+      <c r="L37" s="20"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="21"/>
     </row>
     <row r="38" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="64">
-        <v>194</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>0</v>
+        <v>972</v>
+      </c>
+      <c r="B38" s="48" t="s">
+        <v>1</v>
       </c>
       <c r="C38" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="28"/>
-      <c r="E38" s="24" t="s">
-        <v>23</v>
+      <c r="E38" s="40" t="s">
+        <v>169</v>
       </c>
       <c r="F38" s="23"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="32" t="s">
-        <v>24</v>
+      <c r="G38" s="40"/>
+      <c r="H38" s="56" t="s">
+        <v>170</v>
       </c>
       <c r="I38" s="69" t="s">
-        <v>277</v>
-      </c>
-      <c r="J38" s="26"/>
-      <c r="K38" s="33"/>
+        <v>332</v>
+      </c>
+      <c r="J38" s="41"/>
+      <c r="K38" s="31" t="s">
+        <v>358</v>
+      </c>
       <c r="L38" s="23"/>
       <c r="M38" s="28"/>
       <c r="N38" s="28"/>
@@ -2985,38 +3032,38 @@
     </row>
     <row r="39" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="64">
-        <v>199</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="28"/>
-      <c r="E39" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F39" s="23"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="I39" s="69" t="s">
-        <v>261</v>
-      </c>
-      <c r="J39" s="26"/>
-      <c r="K39" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="L39" s="23"/>
-      <c r="M39" s="28"/>
-      <c r="N39" s="28"/>
-      <c r="O39" s="29"/>
-    </row>
-    <row r="40" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+        <v>975</v>
+      </c>
+      <c r="B39" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="14"/>
+      <c r="E39" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="F39" s="20"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="52" t="s">
+        <v>172</v>
+      </c>
+      <c r="I39" s="68" t="s">
+        <v>333</v>
+      </c>
+      <c r="J39" s="43"/>
+      <c r="K39" s="31" t="s">
+        <v>358</v>
+      </c>
+      <c r="L39" s="20"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="21"/>
+    </row>
+    <row r="40" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="64">
-        <v>202</v>
+        <v>891</v>
       </c>
       <c r="B40" s="13" t="s">
         <v>0</v>
@@ -3026,26 +3073,28 @@
       </c>
       <c r="D40" s="14"/>
       <c r="E40" s="15" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F40" s="20"/>
       <c r="G40" s="15"/>
-      <c r="H40" s="16" t="s">
-        <v>51</v>
+      <c r="H40" s="30" t="s">
+        <v>37</v>
       </c>
       <c r="I40" s="68" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="J40" s="18"/>
-      <c r="K40" s="19"/>
+      <c r="K40" s="19" t="s">
+        <v>38</v>
+      </c>
       <c r="L40" s="20"/>
       <c r="M40" s="14"/>
       <c r="N40" s="14"/>
       <c r="O40" s="21"/>
     </row>
-    <row r="41" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="64">
-        <v>213</v>
+        <v>911</v>
       </c>
       <c r="B41" s="13" t="s">
         <v>0</v>
@@ -3055,78 +3104,76 @@
       </c>
       <c r="D41" s="28"/>
       <c r="E41" s="24" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F41" s="23"/>
       <c r="G41" s="24"/>
-      <c r="H41" s="32" t="s">
-        <v>40</v>
+      <c r="H41" s="25" t="s">
+        <v>34</v>
       </c>
       <c r="I41" s="69" t="s">
-        <v>278</v>
+        <v>325</v>
       </c>
       <c r="J41" s="26"/>
       <c r="K41" s="33" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="L41" s="23"/>
       <c r="M41" s="28"/>
       <c r="N41" s="28"/>
       <c r="O41" s="29"/>
     </row>
-    <row r="42" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="64">
-        <v>214</v>
+        <v>55</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="28"/>
-      <c r="E42" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="F42" s="23"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="I42" s="69" t="s">
-        <v>279</v>
-      </c>
-      <c r="J42" s="26"/>
-      <c r="K42" s="33"/>
-      <c r="L42" s="23"/>
-      <c r="M42" s="28"/>
-      <c r="N42" s="28"/>
-      <c r="O42" s="29"/>
+      <c r="C42" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="14"/>
+      <c r="E42" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="20"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="I42" s="38"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="45"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="21"/>
     </row>
     <row r="43" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="64">
-        <v>216</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>0</v>
+        <v>979</v>
+      </c>
+      <c r="B43" s="48" t="s">
+        <v>1</v>
       </c>
       <c r="C43" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D43" s="28"/>
-      <c r="E43" s="24" t="s">
-        <v>46</v>
+      <c r="E43" s="55" t="s">
+        <v>173</v>
       </c>
       <c r="F43" s="23"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="32" t="s">
-        <v>47</v>
+      <c r="G43" s="55"/>
+      <c r="H43" s="56" t="s">
+        <v>156</v>
       </c>
       <c r="I43" s="69" t="s">
-        <v>263</v>
-      </c>
-      <c r="J43" s="26"/>
-      <c r="K43" s="33"/>
+        <v>319</v>
+      </c>
+      <c r="J43" s="55"/>
+      <c r="K43" s="27"/>
       <c r="L43" s="23"/>
       <c r="M43" s="28"/>
       <c r="N43" s="28"/>
@@ -3134,7 +3181,7 @@
     </row>
     <row r="44" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="64">
-        <v>237</v>
+        <v>59</v>
       </c>
       <c r="B44" s="13" t="s">
         <v>0</v>
@@ -3144,57 +3191,55 @@
       </c>
       <c r="D44" s="28"/>
       <c r="E44" s="24" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="F44" s="23"/>
       <c r="G44" s="24"/>
       <c r="H44" s="25" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="I44" s="69" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="J44" s="26"/>
-      <c r="K44" s="33" t="s">
-        <v>237</v>
-      </c>
+      <c r="K44" s="27"/>
       <c r="L44" s="23"/>
       <c r="M44" s="28"/>
       <c r="N44" s="28"/>
       <c r="O44" s="29"/>
     </row>
-    <row r="45" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="64">
-        <v>2853</v>
-      </c>
-      <c r="B45" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="13"/>
-      <c r="E45" s="58" t="s">
-        <v>52</v>
-      </c>
-      <c r="F45" s="62"/>
-      <c r="G45" s="58"/>
-      <c r="H45" s="59" t="s">
-        <v>53</v>
-      </c>
-      <c r="I45" s="70" t="s">
-        <v>352</v>
-      </c>
-      <c r="J45" s="60"/>
-      <c r="K45" s="61"/>
-      <c r="L45" s="62"/>
-      <c r="M45" s="13"/>
-      <c r="N45" s="13"/>
-      <c r="O45" s="63"/>
-    </row>
-    <row r="46" spans="1:15" customFormat="1" ht="28" x14ac:dyDescent="0.35">
+        <v>983</v>
+      </c>
+      <c r="B45" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="14"/>
+      <c r="E45" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="F45" s="20"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="I45" s="68" t="s">
+        <v>334</v>
+      </c>
+      <c r="J45" s="18"/>
+      <c r="K45" s="31"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="14"/>
+      <c r="O45" s="21"/>
+    </row>
+    <row r="46" spans="1:15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="64">
-        <v>261</v>
+        <v>88</v>
       </c>
       <c r="B46" s="13" t="s">
         <v>0</v>
@@ -3204,28 +3249,26 @@
       </c>
       <c r="D46" s="14"/>
       <c r="E46" s="15" t="s">
-        <v>129</v>
+        <v>227</v>
       </c>
       <c r="F46" s="20"/>
       <c r="G46" s="15"/>
-      <c r="H46" s="16" t="s">
-        <v>130</v>
+      <c r="H46" s="30" t="s">
+        <v>57</v>
       </c>
       <c r="I46" s="68" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
       <c r="J46" s="18"/>
-      <c r="K46" s="19" t="s">
-        <v>359</v>
-      </c>
+      <c r="K46" s="19"/>
       <c r="L46" s="20"/>
       <c r="M46" s="14"/>
       <c r="N46" s="14"/>
       <c r="O46" s="21"/>
     </row>
-    <row r="47" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="64">
-        <v>262</v>
+        <v>93</v>
       </c>
       <c r="B47" s="13" t="s">
         <v>0</v>
@@ -3235,82 +3278,76 @@
       </c>
       <c r="D47" s="14"/>
       <c r="E47" s="15" t="s">
-        <v>131</v>
+        <v>228</v>
       </c>
       <c r="F47" s="20"/>
       <c r="G47" s="15"/>
-      <c r="H47" s="16" t="s">
-        <v>132</v>
+      <c r="H47" s="30" t="s">
+        <v>229</v>
       </c>
       <c r="I47" s="68" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="J47" s="18"/>
-      <c r="K47" s="19" t="s">
-        <v>359</v>
-      </c>
+      <c r="K47" s="19"/>
       <c r="L47" s="20"/>
       <c r="M47" s="14"/>
       <c r="N47" s="14"/>
       <c r="O47" s="21"/>
     </row>
-    <row r="48" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="64">
-        <v>264</v>
+        <v>96</v>
       </c>
       <c r="B48" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C48" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="14"/>
-      <c r="E48" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="F48" s="20"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="I48" s="68" t="s">
-        <v>261</v>
-      </c>
-      <c r="J48" s="18"/>
-      <c r="K48" s="19" t="s">
-        <v>359</v>
-      </c>
-      <c r="L48" s="20"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="21"/>
+      <c r="C48" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="28"/>
+      <c r="E48" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="F48" s="23"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="I48" s="69" t="s">
+        <v>271</v>
+      </c>
+      <c r="J48" s="26"/>
+      <c r="K48" s="33"/>
+      <c r="L48" s="23"/>
+      <c r="M48" s="28"/>
+      <c r="N48" s="28"/>
+      <c r="O48" s="29"/>
     </row>
     <row r="49" spans="1:29" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="64">
-        <v>2895</v>
-      </c>
-      <c r="B49" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="23"/>
+        <v>101</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="28"/>
       <c r="E49" s="24" t="s">
-        <v>219</v>
+        <v>11</v>
       </c>
       <c r="F49" s="23"/>
       <c r="G49" s="24"/>
-      <c r="H49" s="25" t="s">
-        <v>220</v>
+      <c r="H49" s="42" t="s">
+        <v>12</v>
       </c>
       <c r="I49" s="69" t="s">
-        <v>353</v>
+        <v>272</v>
       </c>
       <c r="J49" s="26"/>
-      <c r="K49" s="19" t="s">
-        <v>359</v>
-      </c>
+      <c r="K49" s="33"/>
       <c r="L49" s="23"/>
       <c r="M49" s="28"/>
       <c r="N49" s="28"/>
@@ -3318,65 +3355,61 @@
     </row>
     <row r="50" spans="1:29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="64">
-        <v>271</v>
+        <v>102</v>
       </c>
       <c r="B50" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C50" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="28"/>
-      <c r="E50" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="F50" s="23"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="I50" s="69" t="s">
-        <v>283</v>
-      </c>
-      <c r="J50" s="26"/>
-      <c r="K50" s="19" t="s">
-        <v>359</v>
-      </c>
-      <c r="L50" s="23"/>
-      <c r="M50" s="28"/>
-      <c r="N50" s="28"/>
-      <c r="O50" s="29"/>
-    </row>
-    <row r="51" spans="1:29" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="14"/>
+      <c r="E50" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" s="20"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="68" t="s">
+        <v>273</v>
+      </c>
+      <c r="J50" s="18"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="14"/>
+      <c r="N50" s="14"/>
+      <c r="O50" s="21"/>
+    </row>
+    <row r="51" spans="1:29" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="64">
-        <v>272</v>
-      </c>
-      <c r="B51" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="28"/>
-      <c r="E51" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="F51" s="34"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="I51" s="69" t="s">
-        <v>284</v>
-      </c>
-      <c r="J51" s="26"/>
-      <c r="K51" s="19" t="s">
-        <v>359</v>
-      </c>
-      <c r="L51" s="34"/>
-      <c r="M51" s="28"/>
-      <c r="N51" s="28"/>
-      <c r="O51" s="29"/>
+        <v>1010</v>
+      </c>
+      <c r="B51" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="14"/>
+      <c r="E51" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="F51" s="20"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="I51" s="68" t="s">
+        <v>335</v>
+      </c>
+      <c r="J51" s="18"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="20"/>
+      <c r="M51" s="14"/>
+      <c r="N51" s="14"/>
+      <c r="O51" s="21"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
@@ -3394,30 +3427,28 @@
     </row>
     <row r="52" spans="1:29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="64">
-        <v>274</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>0</v>
+        <v>1012</v>
+      </c>
+      <c r="B52" s="48" t="s">
+        <v>1</v>
       </c>
       <c r="C52" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D52" s="14"/>
       <c r="E52" s="15" t="s">
-        <v>48</v>
+        <v>181</v>
       </c>
       <c r="F52" s="20"/>
       <c r="G52" s="15"/>
       <c r="H52" s="16" t="s">
-        <v>49</v>
+        <v>182</v>
       </c>
       <c r="I52" s="68" t="s">
-        <v>264</v>
+        <v>337</v>
       </c>
       <c r="J52" s="18"/>
-      <c r="K52" s="19" t="s">
-        <v>359</v>
-      </c>
+      <c r="K52" s="19"/>
       <c r="L52" s="20"/>
       <c r="M52" s="14"/>
       <c r="N52" s="14"/>
@@ -3425,7 +3456,7 @@
     </row>
     <row r="53" spans="1:29" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="64">
-        <v>275</v>
+        <v>119</v>
       </c>
       <c r="B53" s="13" t="s">
         <v>0</v>
@@ -3435,20 +3466,18 @@
       </c>
       <c r="D53" s="14"/>
       <c r="E53" s="15" t="s">
-        <v>138</v>
+        <v>15</v>
       </c>
       <c r="F53" s="20"/>
       <c r="G53" s="15"/>
       <c r="H53" s="16" t="s">
-        <v>139</v>
+        <v>16</v>
       </c>
       <c r="I53" s="68" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="J53" s="18"/>
-      <c r="K53" s="19" t="s">
-        <v>359</v>
-      </c>
+      <c r="K53" s="31"/>
       <c r="L53" s="20"/>
       <c r="M53" s="14"/>
       <c r="N53" s="14"/>
@@ -3456,87 +3485,83 @@
     </row>
     <row r="54" spans="1:29" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="64">
-        <v>294</v>
-      </c>
-      <c r="B54" s="13" t="s">
-        <v>0</v>
+        <v>1023</v>
+      </c>
+      <c r="B54" s="48" t="s">
+        <v>1</v>
       </c>
       <c r="C54" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D54" s="28"/>
       <c r="E54" s="24" t="s">
-        <v>145</v>
+        <v>183</v>
       </c>
       <c r="F54" s="23"/>
       <c r="G54" s="24"/>
       <c r="H54" s="32" t="s">
-        <v>37</v>
+        <v>184</v>
       </c>
       <c r="I54" s="69" t="s">
-        <v>265</v>
+        <v>338</v>
       </c>
       <c r="J54" s="26"/>
-      <c r="K54" s="33" t="s">
-        <v>146</v>
-      </c>
+      <c r="K54" s="33"/>
       <c r="L54" s="23"/>
       <c r="M54" s="28"/>
       <c r="N54" s="28"/>
       <c r="O54" s="29"/>
     </row>
-    <row r="55" spans="1:29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="64">
-        <v>318</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="14"/>
-      <c r="E55" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="F55" s="20"/>
-      <c r="G55" s="15"/>
-      <c r="H55" s="30" t="s">
-        <v>239</v>
-      </c>
-      <c r="I55" s="68" t="s">
-        <v>266</v>
-      </c>
-      <c r="J55" s="18"/>
-      <c r="K55" s="19" t="s">
-        <v>240</v>
-      </c>
-      <c r="L55" s="20"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="14"/>
-      <c r="O55" s="21"/>
+        <v>1035</v>
+      </c>
+      <c r="B55" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="28"/>
+      <c r="E55" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="F55" s="23"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="I55" s="69" t="s">
+        <v>339</v>
+      </c>
+      <c r="J55" s="26"/>
+      <c r="K55" s="33"/>
+      <c r="L55" s="23"/>
+      <c r="M55" s="28"/>
+      <c r="N55" s="28"/>
+      <c r="O55" s="29"/>
     </row>
     <row r="56" spans="1:29" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="64">
-        <v>322</v>
-      </c>
-      <c r="B56" s="13" t="s">
-        <v>0</v>
+        <v>1048</v>
+      </c>
+      <c r="B56" s="48" t="s">
+        <v>1</v>
       </c>
       <c r="C56" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="14"/>
       <c r="E56" s="15" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="F56" s="20"/>
       <c r="G56" s="15"/>
       <c r="H56" s="16" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
       <c r="I56" s="68" t="s">
-        <v>286</v>
+        <v>340</v>
       </c>
       <c r="J56" s="18"/>
       <c r="K56" s="19"/>
@@ -3545,9 +3570,9 @@
       <c r="N56" s="14"/>
       <c r="O56" s="21"/>
     </row>
-    <row r="57" spans="1:29" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:29" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="64">
-        <v>324</v>
+        <v>154</v>
       </c>
       <c r="B57" s="13" t="s">
         <v>0</v>
@@ -3557,20 +3582,18 @@
       </c>
       <c r="D57" s="14"/>
       <c r="E57" s="15" t="s">
-        <v>152</v>
+        <v>9</v>
       </c>
       <c r="F57" s="20"/>
       <c r="G57" s="15"/>
-      <c r="H57" s="16" t="s">
-        <v>153</v>
+      <c r="H57" s="46" t="s">
+        <v>10</v>
       </c>
       <c r="I57" s="68" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="J57" s="18"/>
-      <c r="K57" s="19" t="s">
-        <v>154</v>
-      </c>
+      <c r="K57" s="19"/>
       <c r="L57" s="20"/>
       <c r="M57" s="14"/>
       <c r="N57" s="14"/>
@@ -3578,25 +3601,25 @@
     </row>
     <row r="58" spans="1:29" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="64">
-        <v>341</v>
-      </c>
-      <c r="B58" s="13" t="s">
-        <v>0</v>
+        <v>1054</v>
+      </c>
+      <c r="B58" s="48" t="s">
+        <v>1</v>
       </c>
       <c r="C58" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="28"/>
       <c r="E58" s="24" t="s">
-        <v>56</v>
+        <v>189</v>
       </c>
       <c r="F58" s="23"/>
       <c r="G58" s="24"/>
       <c r="H58" s="32" t="s">
-        <v>57</v>
+        <v>190</v>
       </c>
       <c r="I58" s="69" t="s">
-        <v>260</v>
+        <v>341</v>
       </c>
       <c r="J58" s="26"/>
       <c r="K58" s="33"/>
@@ -3607,212 +3630,210 @@
     </row>
     <row r="59" spans="1:29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="64">
-        <v>352</v>
-      </c>
-      <c r="B59" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C59" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D59" s="28"/>
-      <c r="E59" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="F59" s="23"/>
-      <c r="G59" s="24"/>
-      <c r="H59" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="I59" s="69" t="s">
-        <v>287</v>
-      </c>
-      <c r="J59" s="26"/>
-      <c r="K59" s="33"/>
-      <c r="L59" s="23"/>
-      <c r="M59" s="28"/>
-      <c r="N59" s="28"/>
-      <c r="O59" s="29"/>
+        <v>1065</v>
+      </c>
+      <c r="B59" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="14"/>
+      <c r="E59" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="F59" s="20"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="I59" s="68" t="s">
+        <v>342</v>
+      </c>
+      <c r="J59" s="18"/>
+      <c r="K59" s="19"/>
+      <c r="L59" s="20"/>
+      <c r="M59" s="14"/>
+      <c r="N59" s="14"/>
+      <c r="O59" s="21"/>
     </row>
     <row r="60" spans="1:29" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="64">
-        <v>361</v>
-      </c>
-      <c r="B60" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60" s="14"/>
-      <c r="E60" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F60" s="20"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="I60" s="68" t="s">
-        <v>288</v>
-      </c>
-      <c r="J60" s="18"/>
-      <c r="K60" s="19"/>
-      <c r="L60" s="20"/>
-      <c r="M60" s="14"/>
-      <c r="N60" s="14"/>
-      <c r="O60" s="21"/>
+        <v>1090</v>
+      </c>
+      <c r="B60" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="28"/>
+      <c r="E60" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="F60" s="23"/>
+      <c r="G60" s="24"/>
+      <c r="H60" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="I60" s="69" t="s">
+        <v>344</v>
+      </c>
+      <c r="J60" s="26"/>
+      <c r="K60" s="33"/>
+      <c r="L60" s="23"/>
+      <c r="M60" s="28"/>
+      <c r="N60" s="28"/>
+      <c r="O60" s="29"/>
     </row>
     <row r="61" spans="1:29" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="64">
-        <v>379</v>
+        <v>194</v>
       </c>
       <c r="B61" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C61" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="14"/>
-      <c r="E61" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="F61" s="20"/>
-      <c r="G61" s="15"/>
-      <c r="H61" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="I61" s="68" t="s">
-        <v>289</v>
-      </c>
-      <c r="J61" s="18"/>
-      <c r="K61" s="19"/>
-      <c r="L61" s="20"/>
-      <c r="M61" s="14"/>
-      <c r="N61" s="14"/>
-      <c r="O61" s="21"/>
+      <c r="C61" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="28"/>
+      <c r="E61" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F61" s="23"/>
+      <c r="G61" s="24"/>
+      <c r="H61" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="I61" s="69" t="s">
+        <v>277</v>
+      </c>
+      <c r="J61" s="26"/>
+      <c r="K61" s="33"/>
+      <c r="L61" s="23"/>
+      <c r="M61" s="28"/>
+      <c r="N61" s="28"/>
+      <c r="O61" s="29"/>
     </row>
     <row r="62" spans="1:29" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="64">
-        <v>386</v>
+        <v>202</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C62" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" s="28"/>
-      <c r="E62" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="F62" s="23"/>
-      <c r="G62" s="24"/>
-      <c r="H62" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="I62" s="69" t="s">
-        <v>290</v>
-      </c>
-      <c r="J62" s="26"/>
-      <c r="K62" s="33"/>
-      <c r="L62" s="23"/>
-      <c r="M62" s="28"/>
-      <c r="N62" s="28"/>
-      <c r="O62" s="29"/>
+      <c r="C62" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="14"/>
+      <c r="E62" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F62" s="20"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I62" s="68" t="s">
+        <v>262</v>
+      </c>
+      <c r="J62" s="18"/>
+      <c r="K62" s="19"/>
+      <c r="L62" s="20"/>
+      <c r="M62" s="14"/>
+      <c r="N62" s="14"/>
+      <c r="O62" s="21"/>
     </row>
     <row r="63" spans="1:29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="64">
-        <v>394</v>
+        <v>214</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C63" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63" s="14"/>
-      <c r="E63" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="F63" s="20"/>
-      <c r="G63" s="15"/>
-      <c r="H63" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="I63" s="68" t="s">
-        <v>291</v>
-      </c>
-      <c r="J63" s="18"/>
-      <c r="K63" s="19"/>
-      <c r="L63" s="20"/>
-      <c r="M63" s="14"/>
-      <c r="N63" s="14"/>
-      <c r="O63" s="21"/>
-    </row>
-    <row r="64" spans="1:29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C63" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="28"/>
+      <c r="E63" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="F63" s="23"/>
+      <c r="G63" s="24"/>
+      <c r="H63" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="I63" s="69" t="s">
+        <v>279</v>
+      </c>
+      <c r="J63" s="26"/>
+      <c r="K63" s="33"/>
+      <c r="L63" s="23"/>
+      <c r="M63" s="28"/>
+      <c r="N63" s="28"/>
+      <c r="O63" s="29"/>
+    </row>
+    <row r="64" spans="1:29" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="64">
-        <v>3057</v>
-      </c>
-      <c r="B64" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="C64" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="23"/>
+        <v>216</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="28"/>
       <c r="E64" s="24" t="s">
-        <v>232</v>
+        <v>46</v>
       </c>
       <c r="F64" s="23"/>
       <c r="G64" s="24"/>
-      <c r="H64" s="25" t="s">
-        <v>233</v>
+      <c r="H64" s="32" t="s">
+        <v>47</v>
       </c>
       <c r="I64" s="69" t="s">
-        <v>354</v>
-      </c>
-      <c r="J64" s="24"/>
-      <c r="K64" s="33" t="s">
-        <v>234</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="J64" s="26"/>
+      <c r="K64" s="33"/>
       <c r="L64" s="23"/>
-      <c r="M64" s="23"/>
-      <c r="N64" s="23"/>
-      <c r="O64" s="57"/>
-    </row>
-    <row r="65" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M64" s="28"/>
+      <c r="N64" s="28"/>
+      <c r="O64" s="29"/>
+    </row>
+    <row r="65" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="64">
-        <v>400</v>
-      </c>
-      <c r="B65" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C65" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65" s="28"/>
-      <c r="E65" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="F65" s="23"/>
-      <c r="G65" s="24"/>
-      <c r="H65" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="I65" s="69" t="s">
-        <v>292</v>
-      </c>
-      <c r="J65" s="26"/>
-      <c r="K65" s="33"/>
-      <c r="L65" s="23"/>
-      <c r="M65" s="28"/>
-      <c r="N65" s="28"/>
-      <c r="O65" s="29"/>
+        <v>2853</v>
+      </c>
+      <c r="B65" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="13"/>
+      <c r="E65" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="F65" s="62"/>
+      <c r="G65" s="58"/>
+      <c r="H65" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="I65" s="70" t="s">
+        <v>352</v>
+      </c>
+      <c r="J65" s="60"/>
+      <c r="K65" s="61"/>
+      <c r="L65" s="62"/>
+      <c r="M65" s="13"/>
+      <c r="N65" s="13"/>
+      <c r="O65" s="63"/>
     </row>
     <row r="66" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="64">
-        <v>401</v>
+        <v>322</v>
       </c>
       <c r="B66" s="13" t="s">
         <v>0</v>
@@ -3822,15 +3843,15 @@
       </c>
       <c r="D66" s="14"/>
       <c r="E66" s="15" t="s">
-        <v>74</v>
+        <v>149</v>
       </c>
       <c r="F66" s="20"/>
       <c r="G66" s="15"/>
       <c r="H66" s="16" t="s">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="I66" s="68" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="J66" s="18"/>
       <c r="K66" s="19"/>
@@ -3841,125 +3862,123 @@
     </row>
     <row r="67" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="64">
-        <v>425</v>
+        <v>341</v>
       </c>
       <c r="B67" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C67" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67" s="14"/>
-      <c r="E67" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="F67" s="20"/>
-      <c r="G67" s="15"/>
-      <c r="H67" s="16" t="s">
+      <c r="C67" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="28"/>
+      <c r="E67" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F67" s="23"/>
+      <c r="G67" s="24"/>
+      <c r="H67" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="I67" s="68" t="s">
+      <c r="I67" s="69" t="s">
         <v>260</v>
       </c>
-      <c r="J67" s="18"/>
-      <c r="K67" s="19"/>
-      <c r="L67" s="20"/>
-      <c r="M67" s="14"/>
-      <c r="N67" s="14"/>
-      <c r="O67" s="21"/>
+      <c r="J67" s="26"/>
+      <c r="K67" s="33"/>
+      <c r="L67" s="23"/>
+      <c r="M67" s="28"/>
+      <c r="N67" s="28"/>
+      <c r="O67" s="29"/>
     </row>
     <row r="68" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="64">
-        <v>459</v>
+        <v>352</v>
       </c>
       <c r="B68" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C68" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68" s="14"/>
-      <c r="E68" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="F68" s="20"/>
-      <c r="G68" s="15"/>
-      <c r="H68" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="I68" s="68" t="s">
-        <v>293</v>
-      </c>
-      <c r="J68" s="18"/>
-      <c r="K68" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="L68" s="20"/>
-      <c r="M68" s="14"/>
-      <c r="N68" s="14"/>
-      <c r="O68" s="21"/>
+      <c r="C68" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="28"/>
+      <c r="E68" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F68" s="23"/>
+      <c r="G68" s="24"/>
+      <c r="H68" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="I68" s="69" t="s">
+        <v>287</v>
+      </c>
+      <c r="J68" s="26"/>
+      <c r="K68" s="33"/>
+      <c r="L68" s="23"/>
+      <c r="M68" s="28"/>
+      <c r="N68" s="28"/>
+      <c r="O68" s="29"/>
     </row>
     <row r="69" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="64">
-        <v>467</v>
+        <v>361</v>
       </c>
       <c r="B69" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C69" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D69" s="28"/>
-      <c r="E69" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F69" s="23"/>
-      <c r="G69" s="24"/>
-      <c r="H69" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="I69" s="69" t="s">
-        <v>294</v>
-      </c>
-      <c r="J69" s="26"/>
-      <c r="K69" s="33"/>
-      <c r="L69" s="23"/>
-      <c r="M69" s="28"/>
-      <c r="N69" s="28"/>
-      <c r="O69" s="29"/>
+      <c r="C69" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="14"/>
+      <c r="E69" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F69" s="20"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="I69" s="68" t="s">
+        <v>288</v>
+      </c>
+      <c r="J69" s="18"/>
+      <c r="K69" s="19"/>
+      <c r="L69" s="20"/>
+      <c r="M69" s="14"/>
+      <c r="N69" s="14"/>
+      <c r="O69" s="21"/>
     </row>
     <row r="70" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="64">
-        <v>490</v>
+        <v>379</v>
       </c>
       <c r="B70" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C70" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D70" s="28"/>
-      <c r="E70" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="F70" s="23"/>
-      <c r="G70" s="24"/>
-      <c r="H70" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="I70" s="69" t="s">
-        <v>295</v>
-      </c>
-      <c r="J70" s="26"/>
-      <c r="K70" s="33"/>
-      <c r="L70" s="23"/>
-      <c r="M70" s="28"/>
-      <c r="N70" s="28"/>
-      <c r="O70" s="29"/>
+      <c r="C70" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="14"/>
+      <c r="E70" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F70" s="20"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I70" s="68" t="s">
+        <v>289</v>
+      </c>
+      <c r="J70" s="18"/>
+      <c r="K70" s="19"/>
+      <c r="L70" s="20"/>
+      <c r="M70" s="14"/>
+      <c r="N70" s="14"/>
+      <c r="O70" s="21"/>
     </row>
     <row r="71" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="64">
-        <v>511</v>
+        <v>386</v>
       </c>
       <c r="B71" s="13" t="s">
         <v>0</v>
@@ -3969,15 +3988,15 @@
       </c>
       <c r="D71" s="28"/>
       <c r="E71" s="24" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="F71" s="23"/>
       <c r="G71" s="24"/>
       <c r="H71" s="32" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="I71" s="69" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="J71" s="26"/>
       <c r="K71" s="33"/>
@@ -3988,94 +4007,94 @@
     </row>
     <row r="72" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="64">
-        <v>518</v>
+        <v>394</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C72" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D72" s="28"/>
-      <c r="E72" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="F72" s="23"/>
-      <c r="G72" s="24"/>
-      <c r="H72" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="I72" s="69" t="s">
-        <v>297</v>
-      </c>
-      <c r="J72" s="26"/>
-      <c r="K72" s="33"/>
-      <c r="L72" s="23"/>
-      <c r="M72" s="28"/>
-      <c r="N72" s="28"/>
-      <c r="O72" s="29"/>
+      <c r="C72" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="14"/>
+      <c r="E72" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F72" s="20"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="I72" s="68" t="s">
+        <v>291</v>
+      </c>
+      <c r="J72" s="18"/>
+      <c r="K72" s="19"/>
+      <c r="L72" s="20"/>
+      <c r="M72" s="14"/>
+      <c r="N72" s="14"/>
+      <c r="O72" s="21"/>
     </row>
     <row r="73" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="64">
-        <v>523</v>
+        <v>400</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C73" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D73" s="14"/>
-      <c r="E73" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F73" s="20"/>
-      <c r="G73" s="15"/>
-      <c r="H73" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="I73" s="68" t="s">
-        <v>298</v>
-      </c>
-      <c r="J73" s="18"/>
-      <c r="K73" s="19"/>
-      <c r="L73" s="20"/>
-      <c r="M73" s="14"/>
-      <c r="N73" s="14"/>
-      <c r="O73" s="21"/>
+      <c r="C73" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="28"/>
+      <c r="E73" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="F73" s="23"/>
+      <c r="G73" s="24"/>
+      <c r="H73" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="I73" s="69" t="s">
+        <v>292</v>
+      </c>
+      <c r="J73" s="26"/>
+      <c r="K73" s="33"/>
+      <c r="L73" s="23"/>
+      <c r="M73" s="28"/>
+      <c r="N73" s="28"/>
+      <c r="O73" s="29"/>
     </row>
     <row r="74" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="64">
-        <v>550</v>
+        <v>401</v>
       </c>
       <c r="B74" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C74" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D74" s="28"/>
-      <c r="E74" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="F74" s="23"/>
-      <c r="G74" s="24"/>
-      <c r="H74" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="I74" s="69" t="s">
-        <v>299</v>
-      </c>
-      <c r="J74" s="26"/>
-      <c r="K74" s="33"/>
-      <c r="L74" s="23"/>
-      <c r="M74" s="28"/>
-      <c r="N74" s="28"/>
-      <c r="O74" s="29"/>
+      <c r="C74" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" s="14"/>
+      <c r="E74" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F74" s="20"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I74" s="68" t="s">
+        <v>268</v>
+      </c>
+      <c r="J74" s="18"/>
+      <c r="K74" s="19"/>
+      <c r="L74" s="20"/>
+      <c r="M74" s="14"/>
+      <c r="N74" s="14"/>
+      <c r="O74" s="21"/>
     </row>
     <row r="75" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="64">
-        <v>588</v>
+        <v>425</v>
       </c>
       <c r="B75" s="13" t="s">
         <v>0</v>
@@ -4085,15 +4104,15 @@
       </c>
       <c r="D75" s="14"/>
       <c r="E75" s="15" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="F75" s="20"/>
       <c r="G75" s="15"/>
       <c r="H75" s="16" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="I75" s="68" t="s">
-        <v>300</v>
+        <v>260</v>
       </c>
       <c r="J75" s="18"/>
       <c r="K75" s="19"/>
@@ -4104,7 +4123,7 @@
     </row>
     <row r="76" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="64">
-        <v>591</v>
+        <v>467</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>0</v>
@@ -4114,15 +4133,15 @@
       </c>
       <c r="D76" s="28"/>
       <c r="E76" s="24" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="F76" s="23"/>
       <c r="G76" s="24"/>
       <c r="H76" s="32" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="I76" s="69" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="J76" s="26"/>
       <c r="K76" s="33"/>
@@ -4133,36 +4152,36 @@
     </row>
     <row r="77" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="64">
-        <v>612</v>
+        <v>490</v>
       </c>
       <c r="B77" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C77" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D77" s="14"/>
-      <c r="E77" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="F77" s="20"/>
-      <c r="G77" s="15"/>
-      <c r="H77" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="I77" s="68" t="s">
-        <v>302</v>
-      </c>
-      <c r="J77" s="18"/>
-      <c r="K77" s="19"/>
-      <c r="L77" s="20"/>
-      <c r="M77" s="14"/>
-      <c r="N77" s="14"/>
-      <c r="O77" s="21"/>
+      <c r="C77" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D77" s="28"/>
+      <c r="E77" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="F77" s="23"/>
+      <c r="G77" s="24"/>
+      <c r="H77" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="I77" s="69" t="s">
+        <v>295</v>
+      </c>
+      <c r="J77" s="26"/>
+      <c r="K77" s="33"/>
+      <c r="L77" s="23"/>
+      <c r="M77" s="28"/>
+      <c r="N77" s="28"/>
+      <c r="O77" s="29"/>
     </row>
     <row r="78" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="64">
-        <v>613</v>
+        <v>511</v>
       </c>
       <c r="B78" s="13" t="s">
         <v>0</v>
@@ -4172,15 +4191,15 @@
       </c>
       <c r="D78" s="28"/>
       <c r="E78" s="24" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="F78" s="23"/>
       <c r="G78" s="24"/>
       <c r="H78" s="32" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="I78" s="69" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="J78" s="26"/>
       <c r="K78" s="33"/>
@@ -4191,7 +4210,7 @@
     </row>
     <row r="79" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="64">
-        <v>615</v>
+        <v>518</v>
       </c>
       <c r="B79" s="13" t="s">
         <v>0</v>
@@ -4201,15 +4220,15 @@
       </c>
       <c r="D79" s="28"/>
       <c r="E79" s="24" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="F79" s="23"/>
       <c r="G79" s="24"/>
       <c r="H79" s="32" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="I79" s="69" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="J79" s="26"/>
       <c r="K79" s="33"/>
@@ -4218,38 +4237,38 @@
       <c r="N79" s="28"/>
       <c r="O79" s="29"/>
     </row>
-    <row r="80" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="64">
-        <v>3326</v>
-      </c>
-      <c r="B80" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="C80" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D80" s="28"/>
-      <c r="E80" s="24" t="s">
-        <v>217</v>
-      </c>
-      <c r="F80" s="23"/>
-      <c r="G80" s="24"/>
-      <c r="H80" s="25" t="s">
-        <v>218</v>
-      </c>
-      <c r="I80" s="69" t="s">
-        <v>355</v>
-      </c>
-      <c r="J80" s="26"/>
-      <c r="K80" s="27"/>
-      <c r="L80" s="23"/>
-      <c r="M80" s="28"/>
-      <c r="N80" s="28"/>
-      <c r="O80" s="29"/>
+        <v>523</v>
+      </c>
+      <c r="B80" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" s="14"/>
+      <c r="E80" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F80" s="20"/>
+      <c r="G80" s="15"/>
+      <c r="H80" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="I80" s="68" t="s">
+        <v>298</v>
+      </c>
+      <c r="J80" s="18"/>
+      <c r="K80" s="19"/>
+      <c r="L80" s="20"/>
+      <c r="M80" s="14"/>
+      <c r="N80" s="14"/>
+      <c r="O80" s="21"/>
     </row>
     <row r="81" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="64">
-        <v>634</v>
+        <v>550</v>
       </c>
       <c r="B81" s="13" t="s">
         <v>0</v>
@@ -4259,15 +4278,15 @@
       </c>
       <c r="D81" s="28"/>
       <c r="E81" s="24" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="F81" s="23"/>
       <c r="G81" s="24"/>
       <c r="H81" s="32" t="s">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="I81" s="69" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="J81" s="26"/>
       <c r="K81" s="33"/>
@@ -4278,7 +4297,7 @@
     </row>
     <row r="82" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="64">
-        <v>636</v>
+        <v>588</v>
       </c>
       <c r="B82" s="13" t="s">
         <v>0</v>
@@ -4288,15 +4307,15 @@
       </c>
       <c r="D82" s="14"/>
       <c r="E82" s="15" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="F82" s="20"/>
       <c r="G82" s="15"/>
       <c r="H82" s="16" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="I82" s="68" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="J82" s="18"/>
       <c r="K82" s="19"/>
@@ -4305,96 +4324,96 @@
       <c r="N82" s="14"/>
       <c r="O82" s="21"/>
     </row>
-    <row r="83" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="64">
-        <v>3382</v>
-      </c>
-      <c r="B83" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="C83" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D83" s="14"/>
-      <c r="E83" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F83" s="20"/>
-      <c r="G83" s="15"/>
-      <c r="H83" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="I83" s="68" t="s">
-        <v>305</v>
-      </c>
-      <c r="J83" s="18"/>
-      <c r="K83" s="19"/>
-      <c r="L83" s="20"/>
-      <c r="M83" s="14"/>
-      <c r="N83" s="14"/>
-      <c r="O83" s="21"/>
+        <v>591</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C83" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" s="28"/>
+      <c r="E83" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="F83" s="23"/>
+      <c r="G83" s="24"/>
+      <c r="H83" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="I83" s="69" t="s">
+        <v>301</v>
+      </c>
+      <c r="J83" s="26"/>
+      <c r="K83" s="33"/>
+      <c r="L83" s="23"/>
+      <c r="M83" s="28"/>
+      <c r="N83" s="28"/>
+      <c r="O83" s="29"/>
     </row>
     <row r="84" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="64">
-        <v>643</v>
+        <v>612</v>
       </c>
       <c r="B84" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C84" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D84" s="28"/>
-      <c r="E84" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="F84" s="23"/>
-      <c r="G84" s="24"/>
-      <c r="H84" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="I84" s="69" t="s">
-        <v>307</v>
-      </c>
-      <c r="J84" s="26"/>
-      <c r="K84" s="33"/>
-      <c r="L84" s="23"/>
-      <c r="M84" s="28"/>
-      <c r="N84" s="28"/>
-      <c r="O84" s="29"/>
+      <c r="C84" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D84" s="14"/>
+      <c r="E84" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F84" s="20"/>
+      <c r="G84" s="15"/>
+      <c r="H84" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="I84" s="68" t="s">
+        <v>302</v>
+      </c>
+      <c r="J84" s="18"/>
+      <c r="K84" s="19"/>
+      <c r="L84" s="20"/>
+      <c r="M84" s="14"/>
+      <c r="N84" s="14"/>
+      <c r="O84" s="21"/>
     </row>
     <row r="85" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="64">
-        <v>644</v>
+        <v>613</v>
       </c>
       <c r="B85" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C85" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D85" s="14"/>
-      <c r="E85" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="F85" s="20"/>
-      <c r="G85" s="15"/>
-      <c r="H85" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="I85" s="68" t="s">
-        <v>308</v>
-      </c>
-      <c r="J85" s="18"/>
-      <c r="K85" s="19"/>
-      <c r="L85" s="20"/>
-      <c r="M85" s="14"/>
-      <c r="N85" s="14"/>
-      <c r="O85" s="21"/>
+      <c r="C85" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" s="28"/>
+      <c r="E85" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="F85" s="23"/>
+      <c r="G85" s="24"/>
+      <c r="H85" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="I85" s="69" t="s">
+        <v>303</v>
+      </c>
+      <c r="J85" s="26"/>
+      <c r="K85" s="33"/>
+      <c r="L85" s="23"/>
+      <c r="M85" s="28"/>
+      <c r="N85" s="28"/>
+      <c r="O85" s="29"/>
     </row>
     <row r="86" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="64">
-        <v>656</v>
+        <v>615</v>
       </c>
       <c r="B86" s="13" t="s">
         <v>0</v>
@@ -4404,15 +4423,15 @@
       </c>
       <c r="D86" s="28"/>
       <c r="E86" s="24" t="s">
-        <v>243</v>
+        <v>103</v>
       </c>
       <c r="F86" s="23"/>
       <c r="G86" s="24"/>
       <c r="H86" s="32" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="I86" s="69" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="J86" s="26"/>
       <c r="K86" s="33"/>
@@ -4421,63 +4440,59 @@
       <c r="N86" s="28"/>
       <c r="O86" s="29"/>
     </row>
-    <row r="87" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="64">
-        <v>665</v>
-      </c>
-      <c r="B87" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C87" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D87" s="14"/>
-      <c r="E87" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="F87" s="20"/>
-      <c r="G87" s="15"/>
-      <c r="H87" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="I87" s="68" t="s">
-        <v>310</v>
-      </c>
-      <c r="J87" s="18"/>
-      <c r="K87" s="19"/>
-      <c r="L87" s="20"/>
-      <c r="M87" s="14"/>
-      <c r="N87" s="14"/>
-      <c r="O87" s="21"/>
-    </row>
-    <row r="88" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3326</v>
+      </c>
+      <c r="B87" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C87" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" s="28"/>
+      <c r="E87" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="F87" s="23"/>
+      <c r="G87" s="24"/>
+      <c r="H87" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="I87" s="69" t="s">
+        <v>355</v>
+      </c>
+      <c r="J87" s="26"/>
+      <c r="K87" s="27"/>
+      <c r="L87" s="23"/>
+      <c r="M87" s="28"/>
+      <c r="N87" s="28"/>
+      <c r="O87" s="29"/>
+    </row>
+    <row r="88" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="64">
-        <v>2283</v>
-      </c>
-      <c r="B88" s="50" t="s">
-        <v>2</v>
+        <v>634</v>
+      </c>
+      <c r="B88" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="C88" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D88" s="28"/>
       <c r="E88" s="24" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="F88" s="23"/>
       <c r="G88" s="24"/>
-      <c r="H88" s="25" t="s">
-        <v>31</v>
+      <c r="H88" s="32" t="s">
+        <v>29</v>
       </c>
       <c r="I88" s="69" t="s">
-        <v>315</v>
-      </c>
-      <c r="J88" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="K88" s="33" t="s">
-        <v>8</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="J88" s="26"/>
+      <c r="K88" s="33"/>
       <c r="L88" s="23"/>
       <c r="M88" s="28"/>
       <c r="N88" s="28"/>
@@ -4485,65 +4500,65 @@
     </row>
     <row r="89" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="64">
-        <v>693</v>
+        <v>636</v>
       </c>
       <c r="B89" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C89" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D89" s="28"/>
-      <c r="E89" s="24" t="s">
-        <v>115</v>
-      </c>
-      <c r="F89" s="23"/>
-      <c r="G89" s="24"/>
-      <c r="H89" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="I89" s="69" t="s">
-        <v>311</v>
-      </c>
-      <c r="J89" s="26"/>
-      <c r="K89" s="33"/>
-      <c r="L89" s="23"/>
-      <c r="M89" s="28"/>
-      <c r="N89" s="28"/>
-      <c r="O89" s="29"/>
-    </row>
-    <row r="90" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C89" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" s="14"/>
+      <c r="E89" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F89" s="20"/>
+      <c r="G89" s="15"/>
+      <c r="H89" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="I89" s="68" t="s">
+        <v>306</v>
+      </c>
+      <c r="J89" s="18"/>
+      <c r="K89" s="19"/>
+      <c r="L89" s="20"/>
+      <c r="M89" s="14"/>
+      <c r="N89" s="14"/>
+      <c r="O89" s="21"/>
+    </row>
+    <row r="90" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="64">
-        <v>697</v>
-      </c>
-      <c r="B90" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C90" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D90" s="28"/>
-      <c r="E90" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="F90" s="23"/>
-      <c r="G90" s="24"/>
-      <c r="H90" s="32" t="s">
-        <v>118</v>
-      </c>
-      <c r="I90" s="69" t="s">
-        <v>312</v>
-      </c>
-      <c r="J90" s="26"/>
-      <c r="K90" s="33"/>
-      <c r="L90" s="23"/>
-      <c r="M90" s="28"/>
-      <c r="N90" s="28"/>
-      <c r="O90" s="29"/>
+        <v>3382</v>
+      </c>
+      <c r="B90" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" s="14"/>
+      <c r="E90" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F90" s="20"/>
+      <c r="G90" s="15"/>
+      <c r="H90" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="I90" s="68" t="s">
+        <v>305</v>
+      </c>
+      <c r="J90" s="18"/>
+      <c r="K90" s="19"/>
+      <c r="L90" s="20"/>
+      <c r="M90" s="14"/>
+      <c r="N90" s="14"/>
+      <c r="O90" s="21"/>
     </row>
     <row r="91" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="64">
-        <v>698</v>
+        <v>643</v>
       </c>
       <c r="B91" s="13" t="s">
         <v>0</v>
@@ -4553,15 +4568,15 @@
       </c>
       <c r="D91" s="28"/>
       <c r="E91" s="24" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="F91" s="23"/>
       <c r="G91" s="24"/>
       <c r="H91" s="32" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="I91" s="69" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="J91" s="26"/>
       <c r="K91" s="33"/>
@@ -4572,36 +4587,36 @@
     </row>
     <row r="92" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="64">
-        <v>711</v>
+        <v>644</v>
       </c>
       <c r="B92" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C92" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D92" s="28"/>
-      <c r="E92" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="F92" s="23"/>
-      <c r="G92" s="24"/>
-      <c r="H92" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="I92" s="69" t="s">
-        <v>314</v>
-      </c>
-      <c r="J92" s="26"/>
-      <c r="K92" s="33"/>
-      <c r="L92" s="23"/>
-      <c r="M92" s="28"/>
-      <c r="N92" s="28"/>
-      <c r="O92" s="29"/>
+      <c r="C92" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D92" s="14"/>
+      <c r="E92" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F92" s="20"/>
+      <c r="G92" s="15"/>
+      <c r="H92" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="I92" s="68" t="s">
+        <v>308</v>
+      </c>
+      <c r="J92" s="18"/>
+      <c r="K92" s="19"/>
+      <c r="L92" s="20"/>
+      <c r="M92" s="14"/>
+      <c r="N92" s="14"/>
+      <c r="O92" s="21"/>
     </row>
     <row r="93" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="64">
-        <v>712</v>
+        <v>656</v>
       </c>
       <c r="B93" s="13" t="s">
         <v>0</v>
@@ -4611,15 +4626,15 @@
       </c>
       <c r="D93" s="28"/>
       <c r="E93" s="24" t="s">
-        <v>121</v>
+        <v>243</v>
       </c>
       <c r="F93" s="23"/>
       <c r="G93" s="24"/>
       <c r="H93" s="32" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="I93" s="69" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="J93" s="26"/>
       <c r="K93" s="33"/>
@@ -4630,61 +4645,57 @@
     </row>
     <row r="94" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="64">
-        <v>731</v>
+        <v>665</v>
       </c>
       <c r="B94" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C94" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D94" s="28"/>
-      <c r="E94" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="F94" s="23"/>
-      <c r="G94" s="24"/>
-      <c r="H94" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="I94" s="69" t="s">
-        <v>316</v>
-      </c>
-      <c r="J94" s="26"/>
-      <c r="K94" s="33" t="s">
-        <v>124</v>
-      </c>
-      <c r="L94" s="23"/>
-      <c r="M94" s="28"/>
-      <c r="N94" s="28"/>
-      <c r="O94" s="29"/>
-    </row>
-    <row r="95" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C94" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" s="14"/>
+      <c r="E94" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F94" s="20"/>
+      <c r="G94" s="15"/>
+      <c r="H94" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="I94" s="68" t="s">
+        <v>310</v>
+      </c>
+      <c r="J94" s="18"/>
+      <c r="K94" s="19"/>
+      <c r="L94" s="20"/>
+      <c r="M94" s="14"/>
+      <c r="N94" s="14"/>
+      <c r="O94" s="21"/>
+    </row>
+    <row r="95" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="64">
-        <v>3562</v>
-      </c>
-      <c r="B95" s="53" t="s">
-        <v>3</v>
+        <v>693</v>
+      </c>
+      <c r="B95" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="C95" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D95" s="28"/>
       <c r="E95" s="24" t="s">
-        <v>224</v>
+        <v>115</v>
       </c>
       <c r="F95" s="23"/>
       <c r="G95" s="24"/>
-      <c r="H95" s="25" t="s">
-        <v>225</v>
+      <c r="H95" s="32" t="s">
+        <v>116</v>
       </c>
       <c r="I95" s="69" t="s">
-        <v>356</v>
+        <v>311</v>
       </c>
       <c r="J95" s="26"/>
-      <c r="K95" s="33" t="s">
-        <v>226</v>
-      </c>
+      <c r="K95" s="33"/>
       <c r="L95" s="23"/>
       <c r="M95" s="28"/>
       <c r="N95" s="28"/>
@@ -4692,54 +4703,54 @@
     </row>
     <row r="96" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="64">
-        <v>748</v>
+        <v>697</v>
       </c>
       <c r="B96" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C96" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D96" s="14"/>
-      <c r="E96" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="F96" s="20"/>
-      <c r="G96" s="15"/>
-      <c r="H96" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="I96" s="68" t="s">
-        <v>317</v>
-      </c>
-      <c r="J96" s="18"/>
-      <c r="K96" s="19"/>
-      <c r="L96" s="20"/>
-      <c r="M96" s="14"/>
-      <c r="N96" s="14"/>
-      <c r="O96" s="21"/>
-    </row>
-    <row r="97" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C96" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D96" s="28"/>
+      <c r="E96" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="F96" s="23"/>
+      <c r="G96" s="24"/>
+      <c r="H96" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="I96" s="69" t="s">
+        <v>312</v>
+      </c>
+      <c r="J96" s="26"/>
+      <c r="K96" s="33"/>
+      <c r="L96" s="23"/>
+      <c r="M96" s="28"/>
+      <c r="N96" s="28"/>
+      <c r="O96" s="29"/>
+    </row>
+    <row r="97" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="64">
-        <v>2340</v>
-      </c>
-      <c r="B97" s="54" t="s">
-        <v>2</v>
+        <v>698</v>
+      </c>
+      <c r="B97" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="C97" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D97" s="28"/>
       <c r="E97" s="24" t="s">
-        <v>212</v>
+        <v>125</v>
       </c>
       <c r="F97" s="23"/>
       <c r="G97" s="24"/>
-      <c r="H97" s="35" t="s">
-        <v>213</v>
+      <c r="H97" s="32" t="s">
+        <v>126</v>
       </c>
       <c r="I97" s="69" t="s">
-        <v>350</v>
+        <v>313</v>
       </c>
       <c r="J97" s="26"/>
       <c r="K97" s="33"/>
@@ -4750,36 +4761,36 @@
     </row>
     <row r="98" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="64">
-        <v>1637</v>
-      </c>
-      <c r="B98" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="C98" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D98" s="14"/>
-      <c r="E98" s="15" t="s">
-        <v>201</v>
-      </c>
-      <c r="F98" s="20"/>
-      <c r="G98" s="15"/>
-      <c r="H98" s="16" t="s">
-        <v>202</v>
-      </c>
-      <c r="I98" s="68" t="s">
-        <v>346</v>
-      </c>
-      <c r="J98" s="18"/>
-      <c r="K98" s="19"/>
-      <c r="L98" s="20"/>
-      <c r="M98" s="14"/>
-      <c r="N98" s="14"/>
-      <c r="O98" s="21"/>
+        <v>711</v>
+      </c>
+      <c r="B98" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C98" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D98" s="28"/>
+      <c r="E98" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="F98" s="23"/>
+      <c r="G98" s="24"/>
+      <c r="H98" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="I98" s="69" t="s">
+        <v>314</v>
+      </c>
+      <c r="J98" s="26"/>
+      <c r="K98" s="33"/>
+      <c r="L98" s="23"/>
+      <c r="M98" s="28"/>
+      <c r="N98" s="28"/>
+      <c r="O98" s="29"/>
     </row>
     <row r="99" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="64">
-        <v>766</v>
+        <v>712</v>
       </c>
       <c r="B99" s="13" t="s">
         <v>0</v>
@@ -4789,18 +4800,18 @@
       </c>
       <c r="D99" s="28"/>
       <c r="E99" s="24" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="F99" s="23"/>
       <c r="G99" s="24"/>
       <c r="H99" s="32" t="s">
-        <v>134</v>
+        <v>31</v>
       </c>
       <c r="I99" s="69" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="J99" s="26"/>
-      <c r="K99" s="27"/>
+      <c r="K99" s="33"/>
       <c r="L99" s="23"/>
       <c r="M99" s="28"/>
       <c r="N99" s="28"/>
@@ -4808,7 +4819,7 @@
     </row>
     <row r="100" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="64">
-        <v>778</v>
+        <v>748</v>
       </c>
       <c r="B100" s="13" t="s">
         <v>0</v>
@@ -4818,15 +4829,15 @@
       </c>
       <c r="D100" s="14"/>
       <c r="E100" s="15" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="F100" s="20"/>
       <c r="G100" s="15"/>
       <c r="H100" s="16" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="I100" s="68" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="J100" s="18"/>
       <c r="K100" s="19"/>
@@ -4835,27 +4846,27 @@
       <c r="N100" s="14"/>
       <c r="O100" s="21"/>
     </row>
-    <row r="101" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="64">
-        <v>795</v>
-      </c>
-      <c r="B101" s="13" t="s">
-        <v>0</v>
+        <v>2340</v>
+      </c>
+      <c r="B101" s="54" t="s">
+        <v>2</v>
       </c>
       <c r="C101" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D101" s="28"/>
       <c r="E101" s="24" t="s">
-        <v>147</v>
+        <v>212</v>
       </c>
       <c r="F101" s="23"/>
       <c r="G101" s="24"/>
-      <c r="H101" s="32" t="s">
-        <v>148</v>
+      <c r="H101" s="35" t="s">
+        <v>213</v>
       </c>
       <c r="I101" s="69" t="s">
-        <v>320</v>
+        <v>350</v>
       </c>
       <c r="J101" s="26"/>
       <c r="K101" s="33"/>
@@ -4864,38 +4875,38 @@
       <c r="N101" s="28"/>
       <c r="O101" s="29"/>
     </row>
-    <row r="102" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="64">
-        <v>805</v>
-      </c>
-      <c r="B102" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C102" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D102" s="28"/>
-      <c r="E102" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="F102" s="23"/>
-      <c r="G102" s="24"/>
-      <c r="H102" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="I102" s="69" t="s">
-        <v>321</v>
-      </c>
-      <c r="J102" s="26"/>
-      <c r="K102" s="33"/>
-      <c r="L102" s="23"/>
-      <c r="M102" s="28"/>
-      <c r="N102" s="28"/>
-      <c r="O102" s="29"/>
+        <v>1637</v>
+      </c>
+      <c r="B102" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D102" s="14"/>
+      <c r="E102" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="F102" s="20"/>
+      <c r="G102" s="15"/>
+      <c r="H102" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="I102" s="68" t="s">
+        <v>346</v>
+      </c>
+      <c r="J102" s="18"/>
+      <c r="K102" s="19"/>
+      <c r="L102" s="20"/>
+      <c r="M102" s="14"/>
+      <c r="N102" s="14"/>
+      <c r="O102" s="21"/>
     </row>
     <row r="103" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="64">
-        <v>825</v>
+        <v>766</v>
       </c>
       <c r="B103" s="13" t="s">
         <v>0</v>
@@ -4904,21 +4915,19 @@
         <v>5</v>
       </c>
       <c r="D103" s="28"/>
-      <c r="E103" s="44" t="s">
-        <v>140</v>
+      <c r="E103" s="24" t="s">
+        <v>133</v>
       </c>
       <c r="F103" s="23"/>
-      <c r="G103" s="44"/>
+      <c r="G103" s="24"/>
       <c r="H103" s="32" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="I103" s="69" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="J103" s="26"/>
-      <c r="K103" s="33" t="s">
-        <v>142</v>
-      </c>
+      <c r="K103" s="27"/>
       <c r="L103" s="23"/>
       <c r="M103" s="28"/>
       <c r="N103" s="28"/>
@@ -4926,7 +4935,7 @@
     </row>
     <row r="104" spans="1:15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A104" s="64">
-        <v>846</v>
+        <v>778</v>
       </c>
       <c r="B104" s="13" t="s">
         <v>0</v>
@@ -4936,15 +4945,15 @@
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="15" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="F104" s="20"/>
       <c r="G104" s="15"/>
       <c r="H104" s="16" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="I104" s="68" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="J104" s="18"/>
       <c r="K104" s="19"/>
@@ -4955,25 +4964,25 @@
     </row>
     <row r="105" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="64">
-        <v>1708</v>
-      </c>
-      <c r="B105" s="48" t="s">
-        <v>1</v>
+        <v>795</v>
+      </c>
+      <c r="B105" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="C105" s="28" t="s">
         <v>5</v>
       </c>
       <c r="D105" s="28"/>
       <c r="E105" s="24" t="s">
-        <v>203</v>
+        <v>147</v>
       </c>
       <c r="F105" s="23"/>
       <c r="G105" s="24"/>
       <c r="H105" s="32" t="s">
-        <v>204</v>
+        <v>148</v>
       </c>
       <c r="I105" s="69" t="s">
-        <v>347</v>
+        <v>320</v>
       </c>
       <c r="J105" s="26"/>
       <c r="K105" s="33"/>
@@ -4984,56 +4993,54 @@
     </row>
     <row r="106" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="64">
-        <v>891</v>
+        <v>805</v>
       </c>
       <c r="B106" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C106" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D106" s="14"/>
-      <c r="E106" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F106" s="20"/>
-      <c r="G106" s="15"/>
-      <c r="H106" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="I106" s="68" t="s">
-        <v>265</v>
-      </c>
-      <c r="J106" s="18"/>
-      <c r="K106" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="L106" s="20"/>
-      <c r="M106" s="14"/>
-      <c r="N106" s="14"/>
-      <c r="O106" s="21"/>
+      <c r="C106" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" s="28"/>
+      <c r="E106" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F106" s="23"/>
+      <c r="G106" s="24"/>
+      <c r="H106" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="I106" s="69" t="s">
+        <v>321</v>
+      </c>
+      <c r="J106" s="26"/>
+      <c r="K106" s="33"/>
+      <c r="L106" s="23"/>
+      <c r="M106" s="28"/>
+      <c r="N106" s="28"/>
+      <c r="O106" s="29"/>
     </row>
     <row r="107" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="64">
-        <v>1713</v>
-      </c>
-      <c r="B107" s="48" t="s">
-        <v>1</v>
+        <v>846</v>
+      </c>
+      <c r="B107" s="13" t="s">
+        <v>0</v>
       </c>
       <c r="C107" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D107" s="14"/>
       <c r="E107" s="15" t="s">
-        <v>205</v>
+        <v>143</v>
       </c>
       <c r="F107" s="20"/>
       <c r="G107" s="15"/>
       <c r="H107" s="16" t="s">
-        <v>206</v>
+        <v>144</v>
       </c>
       <c r="I107" s="68" t="s">
-        <v>348</v>
+        <v>323</v>
       </c>
       <c r="J107" s="18"/>
       <c r="K107" s="19"/>
@@ -5044,7 +5051,7 @@
     </row>
     <row r="108" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="64">
-        <v>1714</v>
+        <v>1708</v>
       </c>
       <c r="B108" s="48" t="s">
         <v>1</v>
@@ -5054,20 +5061,18 @@
       </c>
       <c r="D108" s="28"/>
       <c r="E108" s="24" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F108" s="23"/>
       <c r="G108" s="24"/>
       <c r="H108" s="32" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="I108" s="69" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="J108" s="26"/>
-      <c r="K108" s="33" t="s">
-        <v>209</v>
-      </c>
+      <c r="K108" s="33"/>
       <c r="L108" s="23"/>
       <c r="M108" s="28"/>
       <c r="N108" s="28"/>
@@ -5075,57 +5080,57 @@
     </row>
     <row r="109" spans="1:15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="64">
-        <v>5036</v>
-      </c>
-      <c r="B109" s="49" t="s">
-        <v>4</v>
+        <v>1713</v>
+      </c>
+      <c r="B109" s="48" t="s">
+        <v>1</v>
       </c>
       <c r="C109" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D109" s="14"/>
-      <c r="E109" s="36" t="s">
-        <v>241</v>
+      <c r="E109" s="15" t="s">
+        <v>205</v>
       </c>
       <c r="F109" s="20"/>
-      <c r="G109" s="36"/>
-      <c r="H109" s="52" t="s">
-        <v>242</v>
+      <c r="G109" s="15"/>
+      <c r="H109" s="16" t="s">
+        <v>206</v>
       </c>
       <c r="I109" s="68" t="s">
-        <v>357</v>
-      </c>
-      <c r="J109" s="39"/>
-      <c r="K109" s="47"/>
+        <v>348</v>
+      </c>
+      <c r="J109" s="18"/>
+      <c r="K109" s="19"/>
       <c r="L109" s="20"/>
       <c r="M109" s="14"/>
       <c r="N109" s="14"/>
       <c r="O109" s="21"/>
     </row>
-    <row r="110" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="64">
-        <v>906</v>
-      </c>
-      <c r="B110" s="13" t="s">
-        <v>0</v>
+        <v>5036</v>
+      </c>
+      <c r="B110" s="49" t="s">
+        <v>4</v>
       </c>
       <c r="C110" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D110" s="14"/>
-      <c r="E110" s="15" t="s">
-        <v>72</v>
+      <c r="E110" s="36" t="s">
+        <v>241</v>
       </c>
       <c r="F110" s="20"/>
-      <c r="G110" s="15"/>
-      <c r="H110" s="30" t="s">
-        <v>73</v>
+      <c r="G110" s="36"/>
+      <c r="H110" s="52" t="s">
+        <v>242</v>
       </c>
       <c r="I110" s="68" t="s">
-        <v>324</v>
-      </c>
-      <c r="J110" s="18"/>
-      <c r="K110" s="19"/>
+        <v>357</v>
+      </c>
+      <c r="J110" s="39"/>
+      <c r="K110" s="47"/>
       <c r="L110" s="20"/>
       <c r="M110" s="14"/>
       <c r="N110" s="14"/>
@@ -5133,39 +5138,37 @@
     </row>
     <row r="111" spans="1:15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="64">
-        <v>911</v>
+        <v>906</v>
       </c>
       <c r="B111" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C111" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D111" s="28"/>
-      <c r="E111" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="F111" s="23"/>
-      <c r="G111" s="24"/>
-      <c r="H111" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="I111" s="69" t="s">
-        <v>325</v>
-      </c>
-      <c r="J111" s="26"/>
-      <c r="K111" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="L111" s="23"/>
-      <c r="M111" s="28"/>
-      <c r="N111" s="28"/>
-      <c r="O111" s="29"/>
+      <c r="C111" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D111" s="14"/>
+      <c r="E111" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F111" s="20"/>
+      <c r="G111" s="15"/>
+      <c r="H111" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I111" s="68" t="s">
+        <v>324</v>
+      </c>
+      <c r="J111" s="18"/>
+      <c r="K111" s="19"/>
+      <c r="L111" s="20"/>
+      <c r="M111" s="14"/>
+      <c r="N111" s="14"/>
+      <c r="O111" s="21"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:O111" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O111">
-      <sortCondition ref="E1:E111"/>
+      <sortCondition ref="K1:K111"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -5173,7 +5176,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{806D3E86-CA67-4AF6-A231-4A597B5AC0DC}"/>
+    <hyperlink ref="F30" r:id="rId1" xr:uid="{806D3E86-CA67-4AF6-A231-4A597B5AC0DC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>